<commit_message>
Revert 'cards' to commit 95cda46ab8 (Jun 25)
</commit_message>
<xml_diff>
--- a/cards/account_type/account_type.xlsx
+++ b/cards/account_type/account_type.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,70 +440,146 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>_airbyte_ab_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>_airbyte_emitted_at</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>aty_code</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>aty_labe</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>_airbyte_additional_properties</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>source_file_path</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>updated_at</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ad969c63-4ef2-45c3-847b-85f002584c88</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>45510.3079196875</v>
+      </c>
+      <c r="C2" t="n">
         <v>2</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Credit</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>45511.29223457176</v>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>s3a://ai360nica/data/bronze/oracle/eftswitch/MXP/ACCOUNT_TYPE/2024_08_06_1722929004063_1.parquet</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>45511.29223457264</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>4a38db5d-dc2e-4eea-888a-78c6c3b94f6a</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>45510.3079196875</v>
+      </c>
+      <c r="C3" t="n">
         <v>3</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Charge</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>45511.29223457176</v>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>s3a://ai360nica/data/bronze/oracle/eftswitch/MXP/ACCOUNT_TYPE/2024_08_06_1722929004063_1.parquet</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>45511.29223457264</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cae9d427-1b55-4414-9544-9f50c1d392c1</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>45510.3079196875</v>
+      </c>
+      <c r="C4" t="n">
         <v>4</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Pre-Paid</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>45511.29223457176</v>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>s3a://ai360nica/data/bronze/oracle/eftswitch/MXP/ACCOUNT_TYPE/2024_08_06_1722929004063_1.parquet</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>45511.29223457264</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>959f9db3-5a06-4bb9-8b88-96498171a321</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>45510.3079196875</v>
+      </c>
+      <c r="C5" t="n">
         <v>1</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Debit</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>45511.29223457176</v>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>s3a://ai360nica/data/bronze/oracle/eftswitch/MXP/ACCOUNT_TYPE/2024_08_06_1722929004063_0.parquet</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>45511.29223457264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>